<commit_message>
update to tanzania files; adjust discount rate for reportvalues test; no calculation suite
git-svn-id: https://svn.fao.org/projects/ruralinvest/RIV4/trunk@67196 d7fa552c-c32d-11e1-9f2d-6d39f2a56844
</commit_message>
<xml_diff>
--- a/RIV4-tests/src/test/resources/imports/project/Tanzania/projectCashFlowFirst.xlsx
+++ b/RIV4-tests/src/test/resources/imports/project/Tanzania/projectCashFlowFirst.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Cash Flow 1st yr" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
-    <t>Cash flow (first year)</t>
-  </si>
-  <si>
     <t>Jan</t>
   </si>
   <si>
@@ -91,6 +88,10 @@
   </si>
   <si>
     <t>Cumulative cash flow</t>
+  </si>
+  <si>
+    <t>Cash flow (first year) (With project)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -484,7 +485,9 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
@@ -499,58 +502,58 @@
   <sheetData>
     <row r="1" spans="1:14" ht="25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="18">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -595,7 +598,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
@@ -640,12 +643,12 @@
     </row>
     <row r="7" spans="1:14" ht="18">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="4">
         <v>65642.1875</v>
@@ -690,7 +693,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
@@ -735,12 +738,12 @@
     </row>
     <row r="11" spans="1:14" ht="18">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="4">
         <v>2943.5625</v>
@@ -785,7 +788,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="4">
         <v>7330.2624999999998</v>
@@ -830,7 +833,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="4">
         <f t="shared" ref="B14:N14" si="0">SUM(B12:B13)</f>
@@ -887,7 +890,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="4">
         <f t="shared" ref="B15:N15" si="1">SUM(B4:B5)-SUM(B8:B9)-B14</f>
@@ -944,7 +947,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="4">
         <f>B15</f>

</xml_diff>